<commit_message>
I add new value.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -384,6 +384,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>